<commit_message>
Comparing original (real) with synthesized data
</commit_message>
<xml_diff>
--- a/insurance.xlsx
+++ b/insurance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B782401-7255-4A3B-B3F6-49C917AFF7AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9B75EA-C3F1-45E4-A1EA-A9B29C9684E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,19 +21,11 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Original!$G$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Original!$G$2:$G$1339</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Original!$A$1</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Original!$A$2:$A$1339</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Original!$C$1</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Original!$C$2:$C$1339</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Original!$A$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Original!$A$2:$A$1339</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Original!$G$1</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Original!$G$2:$G$1339</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Mostly.AI!$G$1</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Mostly.AI!$G$2:$G$1339</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Original!$C$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Original!$C$2:$C$1339</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Original!$A$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Original!$A$2:$A$1339</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Mostly.AI!$G$1</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Mostly.AI!$G$1</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Mostly.AI!$G$2:$G$1339</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Mostly.AI!$G$2:$G$1339</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Mostly.AI!$G$1</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Mostly.AI!$G$2:$G$1339</definedName>
@@ -60,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12077" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12079" uniqueCount="31">
   <si>
     <t>age</t>
   </si>
@@ -148,6 +140,12 @@
   <si>
     <t>Stdev children</t>
   </si>
+  <si>
+    <t>Max charge*</t>
+  </si>
+  <si>
+    <t>* This feature has a bimodal distribution</t>
+  </si>
 </sst>
 </file>
 
@@ -156,7 +154,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,6 +285,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -639,13 +643,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -93450,10 +93455,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B89465A6-4E2A-4EF8-BD5A-71A373B42F0F}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -93563,104 +93568,126 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6">
+        <f>MAX(Original!G:G)</f>
+        <v>63770.428010000003</v>
+      </c>
+      <c r="C7" s="6">
+        <f>MAX(Mostly.AI!G:G)</f>
+        <v>49993.107000000004</v>
+      </c>
+      <c r="D7" s="6">
+        <f>MAX(VGranville!G:G)</f>
+        <v>59588.126568549204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="3">
         <f>CORREL(Original!A:A,Original!C:C)</f>
         <v>0.10927188154853502</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C8" s="3">
         <f>CORREL(Mostly.AI!A:A,Mostly.AI!C:C)</f>
         <v>5.5368413190186781E-2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D8" s="3">
         <f>CORREL(VGranville!D:D,VGranville!E:E)</f>
         <v>8.9984872482160305E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <f>CORREL(Original!A:A,Original!D:D)</f>
         <v>4.2468998558849488E-2</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C9" s="3">
         <f>CORREL(Mostly.AI!A:A,Mostly.AI!D:D)</f>
         <v>2.1300408644591748E-2</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D9" s="3">
         <f>CORREL(VGranville!D:D,VGranville!F:F)</f>
         <v>2.5906109742855787E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <f>CORREL(Original!A:A,Original!G:G)</f>
         <v>0.29900819333064782</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C10" s="3">
         <f>CORREL(Mostly.AI!A:A,Mostly.AI!G:G)</f>
         <v>0.29383528192775055</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D10" s="3">
         <f>CORREL(VGranville!D:D,VGranville!G:G)</f>
         <v>0.30000261083960778</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="3">
         <f>CORREL(Original!C:C,Original!G:G)</f>
         <v>0.19834096883362906</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C11" s="3">
         <f>CORREL(Mostly.AI!C:C,Mostly.AI!G:G)</f>
         <v>0.1404591244253206</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D11" s="3">
         <f>CORREL(VGranville!E:E,VGranville!G:G)</f>
         <v>0.18146555042122775</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <f>STDEV(Original!D:D)</f>
         <v>1.2054927397819137</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <f>STDEV(Mostly.AI!D:D)</f>
         <v>1.1936797735788218</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <f>STDEV(VGranville!F:F)</f>
         <v>1.1989811878216048</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="4">
         <f>STDEV(Original!G:G)</f>
         <v>12110.01123669401</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C13" s="4">
         <f>STDEV(Mostly.AI!G:G)</f>
         <v>12330.304555302118</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D13" s="4">
         <f>STDEV(VGranville!G:G)</f>
         <v>12132.205037379919</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>